<commit_message>
update at 01:18 on 10 Mar 2020
</commit_message>
<xml_diff>
--- a/cases-confirmed-by-local-authorities.xlsx
+++ b/cases-confirmed-by-local-authorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xshaun/GitHub/COVID-19-UK/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8950F359-71C5-DC47-96E4-504CBA28FCD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D869614-9F01-D848-9055-8AE3CB8ACCFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27720" windowHeight="17540" xr2:uid="{03FAC37E-E114-B94A-90DB-A205D9B9D727}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="164">
   <si>
     <t>Local authority</t>
   </si>
@@ -522,6 +522,9 @@
   </si>
   <si>
     <t>9:00am on 8 March 2020</t>
+  </si>
+  <si>
+    <t>9:00am on 9 March 2020</t>
   </si>
 </sst>
 </file>
@@ -571,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -584,6 +587,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -899,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E24FA156-A3A6-9444-8142-DD1738F7E1B2}">
-  <dimension ref="A1:F155"/>
+  <dimension ref="A1:H155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:H155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -913,10 +919,11 @@
     <col min="4" max="4" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" style="1" customWidth="1"/>
     <col min="6" max="6" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="16.5" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -935,8 +942,14 @@
       <c r="F1" s="2" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G1" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -955,8 +968,14 @@
       <c r="F2" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -975,8 +994,14 @@
       <c r="F3" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -995,8 +1020,14 @@
       <c r="F4" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="G4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1015,8 +1046,14 @@
       <c r="F5" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1035,8 +1072,14 @@
       <c r="F6" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1055,8 +1098,14 @@
       <c r="F7" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1075,8 +1124,14 @@
       <c r="F8" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1095,8 +1150,14 @@
       <c r="F9" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1115,8 +1176,14 @@
       <c r="F10" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1135,8 +1202,14 @@
       <c r="F11" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="G11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1155,8 +1228,14 @@
       <c r="F12" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G12" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="H12" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1175,8 +1254,14 @@
       <c r="F13" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1195,8 +1280,14 @@
       <c r="F14" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1215,8 +1306,14 @@
       <c r="F15" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1235,8 +1332,14 @@
       <c r="F16" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -1255,8 +1358,14 @@
       <c r="F17" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -1275,8 +1384,14 @@
       <c r="F18" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
@@ -1295,8 +1410,14 @@
       <c r="F19" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G19" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -1315,8 +1436,14 @@
       <c r="F20" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
@@ -1335,8 +1462,14 @@
       <c r="F21" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
@@ -1355,8 +1488,14 @@
       <c r="F22" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
@@ -1375,8 +1514,14 @@
       <c r="F23" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
@@ -1395,8 +1540,14 @@
       <c r="F24" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>25</v>
       </c>
@@ -1415,8 +1566,14 @@
       <c r="F25" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="G25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
@@ -1435,8 +1592,14 @@
       <c r="F26" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G26" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>27</v>
       </c>
@@ -1447,8 +1610,14 @@
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="G27" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="H27" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
@@ -1467,8 +1636,14 @@
       <c r="F28" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G28" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H28" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>29</v>
       </c>
@@ -1487,8 +1662,14 @@
       <c r="F29" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G29" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H29" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>30</v>
       </c>
@@ -1507,8 +1688,14 @@
       <c r="F30" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G30" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
@@ -1527,8 +1714,14 @@
       <c r="F31" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G31" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H31" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>32</v>
       </c>
@@ -1547,8 +1740,14 @@
       <c r="F32" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G32" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H32" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>33</v>
       </c>
@@ -1567,8 +1766,14 @@
       <c r="F33" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G33" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H33" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
@@ -1587,8 +1792,14 @@
       <c r="F34" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G34" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H34" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>35</v>
       </c>
@@ -1607,8 +1818,14 @@
       <c r="F35" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G35" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H35" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>36</v>
       </c>
@@ -1627,8 +1844,14 @@
       <c r="F36" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G36" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H36" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>37</v>
       </c>
@@ -1647,8 +1870,14 @@
       <c r="F37" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G37" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H37" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>38</v>
       </c>
@@ -1667,8 +1896,14 @@
       <c r="F38" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G38" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H38" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>39</v>
       </c>
@@ -1687,8 +1922,14 @@
       <c r="F39" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G39" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H39" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>40</v>
       </c>
@@ -1707,8 +1948,14 @@
       <c r="F40" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G40" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H40" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>41</v>
       </c>
@@ -1727,8 +1974,14 @@
       <c r="F41" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G41" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H41" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>42</v>
       </c>
@@ -1747,8 +2000,14 @@
       <c r="F42" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G42" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H42" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>43</v>
       </c>
@@ -1767,8 +2026,14 @@
       <c r="F43" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G43" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H43" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>44</v>
       </c>
@@ -1787,8 +2052,14 @@
       <c r="F44" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G44" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H44" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>45</v>
       </c>
@@ -1807,8 +2078,14 @@
       <c r="F45" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G45" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H45" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>46</v>
       </c>
@@ -1827,8 +2104,14 @@
       <c r="F46" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G46" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H46" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>47</v>
       </c>
@@ -1847,8 +2130,14 @@
       <c r="F47" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="G47" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="H47" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>48</v>
       </c>
@@ -1867,8 +2156,14 @@
       <c r="F48" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G48" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H48" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>49</v>
       </c>
@@ -1887,8 +2182,14 @@
       <c r="F49" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="G49" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H49" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>50</v>
       </c>
@@ -1907,8 +2208,14 @@
       <c r="F50" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G50" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H50" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>51</v>
       </c>
@@ -1927,8 +2234,14 @@
       <c r="F51" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G51" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H51" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>52</v>
       </c>
@@ -1947,8 +2260,14 @@
       <c r="F52" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G52" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H52" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>53</v>
       </c>
@@ -1967,8 +2286,14 @@
       <c r="F53" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G53" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H53" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>54</v>
       </c>
@@ -1987,8 +2312,14 @@
       <c r="F54" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G54" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H54" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>55</v>
       </c>
@@ -2007,8 +2338,14 @@
       <c r="F55" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G55" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H55" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>56</v>
       </c>
@@ -2027,8 +2364,14 @@
       <c r="F56" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G56" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H56" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>57</v>
       </c>
@@ -2047,8 +2390,14 @@
       <c r="F57" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G57" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H57" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>58</v>
       </c>
@@ -2067,8 +2416,14 @@
       <c r="F58" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G58" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H58" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>59</v>
       </c>
@@ -2087,8 +2442,14 @@
       <c r="F59" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G59" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H59" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>60</v>
       </c>
@@ -2107,8 +2468,14 @@
       <c r="F60" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G60" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H60" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>61</v>
       </c>
@@ -2119,8 +2486,14 @@
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
-    </row>
-    <row r="62" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G61" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H61" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>62</v>
       </c>
@@ -2139,8 +2512,14 @@
       <c r="F62" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G62" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H62" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>63</v>
       </c>
@@ -2159,8 +2538,14 @@
       <c r="F63" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G63" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H63" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>64</v>
       </c>
@@ -2179,8 +2564,14 @@
       <c r="F64" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="G64" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H64" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>65</v>
       </c>
@@ -2199,8 +2590,14 @@
       <c r="F65" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G65" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H65" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>66</v>
       </c>
@@ -2219,8 +2616,14 @@
       <c r="F66" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G66" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H66" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>67</v>
       </c>
@@ -2239,8 +2642,14 @@
       <c r="F67" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G67" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H67" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>68</v>
       </c>
@@ -2259,8 +2668,14 @@
       <c r="F68" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G68" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H68" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>69</v>
       </c>
@@ -2279,8 +2694,14 @@
       <c r="F69" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G69" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H69" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>70</v>
       </c>
@@ -2299,8 +2720,14 @@
       <c r="F70" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G70" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H70" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>71</v>
       </c>
@@ -2319,8 +2746,14 @@
       <c r="F71" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G71" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H71" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>72</v>
       </c>
@@ -2339,8 +2772,14 @@
       <c r="F72" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G72" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H72" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>73</v>
       </c>
@@ -2359,8 +2798,14 @@
       <c r="F73" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G73" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H73" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>74</v>
       </c>
@@ -2379,8 +2824,14 @@
       <c r="F74" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G74" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H74" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>75</v>
       </c>
@@ -2399,8 +2850,14 @@
       <c r="F75" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G75" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H75" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>76</v>
       </c>
@@ -2419,8 +2876,14 @@
       <c r="F76" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G76" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H76" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>77</v>
       </c>
@@ -2439,8 +2902,14 @@
       <c r="F77" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G77" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H77" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>78</v>
       </c>
@@ -2459,8 +2928,14 @@
       <c r="F78" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G78" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H78" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>79</v>
       </c>
@@ -2479,8 +2954,14 @@
       <c r="F79" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G79" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H79" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>80</v>
       </c>
@@ -2499,8 +2980,14 @@
       <c r="F80" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G80" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H80" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>81</v>
       </c>
@@ -2519,8 +3006,14 @@
       <c r="F81" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G81" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H81" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>82</v>
       </c>
@@ -2539,8 +3032,14 @@
       <c r="F82" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G82" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H82" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>83</v>
       </c>
@@ -2559,8 +3058,14 @@
       <c r="F83" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G83" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H83" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>84</v>
       </c>
@@ -2579,8 +3084,14 @@
       <c r="F84" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G84" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H84" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>85</v>
       </c>
@@ -2599,8 +3110,14 @@
       <c r="F85" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G85" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H85" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>86</v>
       </c>
@@ -2619,8 +3136,14 @@
       <c r="F86" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G86" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H86" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>87</v>
       </c>
@@ -2639,8 +3162,14 @@
       <c r="F87" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G87" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H87" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>88</v>
       </c>
@@ -2659,8 +3188,14 @@
       <c r="F88" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G88" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H88" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>89</v>
       </c>
@@ -2679,8 +3214,14 @@
       <c r="F89" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G89" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H89" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>90</v>
       </c>
@@ -2699,8 +3240,14 @@
       <c r="F90" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G90" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H90" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>91</v>
       </c>
@@ -2719,8 +3266,14 @@
       <c r="F91" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G91" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H91" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>92</v>
       </c>
@@ -2739,8 +3292,14 @@
       <c r="F92" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G92" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H92" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>93</v>
       </c>
@@ -2759,8 +3318,14 @@
       <c r="F93" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G93" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H93" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>94</v>
       </c>
@@ -2779,8 +3344,14 @@
       <c r="F94" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G94" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H94" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>95</v>
       </c>
@@ -2799,8 +3370,14 @@
       <c r="F95" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G95" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H95" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>96</v>
       </c>
@@ -2819,8 +3396,14 @@
       <c r="F96" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G96" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H96" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>97</v>
       </c>
@@ -2839,8 +3422,14 @@
       <c r="F97" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G97" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="H97" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>98</v>
       </c>
@@ -2859,8 +3448,14 @@
       <c r="F98" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G98" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H98" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>99</v>
       </c>
@@ -2875,8 +3470,14 @@
       </c>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
-    </row>
-    <row r="100" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G99" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H99" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>100</v>
       </c>
@@ -2895,8 +3496,14 @@
       <c r="F100" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G100" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H100" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>101</v>
       </c>
@@ -2915,8 +3522,14 @@
       <c r="F101" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G101" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="H101" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>102</v>
       </c>
@@ -2935,8 +3548,14 @@
       <c r="F102" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G102" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H102" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>103</v>
       </c>
@@ -2955,8 +3574,14 @@
       <c r="F103" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G103" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H103" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>104</v>
       </c>
@@ -2975,8 +3600,14 @@
       <c r="F104" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G104" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="H104" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>105</v>
       </c>
@@ -2995,8 +3626,14 @@
       <c r="F105" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G105" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="H105" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>106</v>
       </c>
@@ -3015,8 +3652,14 @@
       <c r="F106" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G106" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="H106" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>107</v>
       </c>
@@ -3035,8 +3678,14 @@
       <c r="F107" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G107" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="H107" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>108</v>
       </c>
@@ -3055,8 +3704,14 @@
       <c r="F108" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G108" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="H108" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>109</v>
       </c>
@@ -3075,8 +3730,14 @@
       <c r="F109" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G109" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="H109" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>110</v>
       </c>
@@ -3095,8 +3756,14 @@
       <c r="F110" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G110" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="H110" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>111</v>
       </c>
@@ -3115,8 +3782,14 @@
       <c r="F111" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G111" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H111" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>112</v>
       </c>
@@ -3135,8 +3808,14 @@
       <c r="F112" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G112" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H112" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>113</v>
       </c>
@@ -3155,8 +3834,14 @@
       <c r="F113" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G113" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H113" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>114</v>
       </c>
@@ -3175,8 +3860,14 @@
       <c r="F114" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G114" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="H114" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>115</v>
       </c>
@@ -3195,8 +3886,14 @@
       <c r="F115" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G115" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H115" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>116</v>
       </c>
@@ -3215,8 +3912,14 @@
       <c r="F116" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G116" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="H116" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>117</v>
       </c>
@@ -3235,8 +3938,14 @@
       <c r="F117" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G117" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H117" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>118</v>
       </c>
@@ -3255,8 +3964,14 @@
       <c r="F118" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G118" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="H118" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>119</v>
       </c>
@@ -3275,8 +3990,14 @@
       <c r="F119" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G119" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H119" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>120</v>
       </c>
@@ -3295,8 +4016,14 @@
       <c r="F120" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G120" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="H120" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>121</v>
       </c>
@@ -3315,8 +4042,14 @@
       <c r="F121" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G121" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="H121" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>122</v>
       </c>
@@ -3335,8 +4068,14 @@
       <c r="F122" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G122" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="H122" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>123</v>
       </c>
@@ -3355,8 +4094,14 @@
       <c r="F123" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G123" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="H123" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>124</v>
       </c>
@@ -3375,8 +4120,14 @@
       <c r="F124" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G124" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H124" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>125</v>
       </c>
@@ -3395,8 +4146,14 @@
       <c r="F125" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G125" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="H125" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>126</v>
       </c>
@@ -3415,8 +4172,14 @@
       <c r="F126" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G126" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H126" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>127</v>
       </c>
@@ -3435,8 +4198,14 @@
       <c r="F127" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G127" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="H127" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>128</v>
       </c>
@@ -3455,8 +4224,14 @@
       <c r="F128" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G128" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="H128" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>129</v>
       </c>
@@ -3475,8 +4250,14 @@
       <c r="F129" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G129" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="H129" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>130</v>
       </c>
@@ -3495,8 +4276,14 @@
       <c r="F130" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G130" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="H130" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>131</v>
       </c>
@@ -3515,8 +4302,14 @@
       <c r="F131" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G131" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H131" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>132</v>
       </c>
@@ -3535,8 +4328,14 @@
       <c r="F132" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G132" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="H132" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>133</v>
       </c>
@@ -3555,8 +4354,14 @@
       <c r="F133" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G133" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="H133" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>134</v>
       </c>
@@ -3575,8 +4380,14 @@
       <c r="F134" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G134" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H134" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>135</v>
       </c>
@@ -3595,8 +4406,14 @@
       <c r="F135" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G135" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H135" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>136</v>
       </c>
@@ -3615,8 +4432,14 @@
       <c r="F136" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G136" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="H136" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>137</v>
       </c>
@@ -3635,8 +4458,14 @@
       <c r="F137" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G137" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H137" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>138</v>
       </c>
@@ -3655,8 +4484,14 @@
       <c r="F138" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G138" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="H138" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>139</v>
       </c>
@@ -3675,8 +4510,14 @@
       <c r="F139" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G139" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="H139" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>140</v>
       </c>
@@ -3695,8 +4536,14 @@
       <c r="F140" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G140" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="H140" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>141</v>
       </c>
@@ -3715,8 +4562,14 @@
       <c r="F141" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G141" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="H141" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>142</v>
       </c>
@@ -3735,8 +4588,14 @@
       <c r="F142" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G142" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="H142" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>143</v>
       </c>
@@ -3755,8 +4614,14 @@
       <c r="F143" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G143" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="H143" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>144</v>
       </c>
@@ -3775,8 +4640,14 @@
       <c r="F144" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G144" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="H144" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>145</v>
       </c>
@@ -3795,8 +4666,14 @@
       <c r="F145" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G145" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="H145" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>146</v>
       </c>
@@ -3815,8 +4692,14 @@
       <c r="F146" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G146" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="H146" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>147</v>
       </c>
@@ -3835,8 +4718,14 @@
       <c r="F147" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="G147" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="H147" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>148</v>
       </c>
@@ -3855,8 +4744,14 @@
       <c r="F148" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G148" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="H148" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>149</v>
       </c>
@@ -3875,8 +4770,14 @@
       <c r="F149" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="150" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G149" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="H149" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>150</v>
       </c>
@@ -3895,8 +4796,14 @@
       <c r="F150" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G150" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="H150" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>151</v>
       </c>
@@ -3915,8 +4822,14 @@
       <c r="F151" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G151" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="H151" s="5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>152</v>
       </c>
@@ -3936,7 +4849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>153</v>
       </c>
@@ -3956,7 +4869,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>154</v>
       </c>
@@ -3976,7 +4889,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" s="3"/>
       <c r="B155" s="3"/>
       <c r="C155" s="3"/>

</xml_diff>

<commit_message>
update at 07:54 on 11 Mar 2020
</commit_message>
<xml_diff>
--- a/cases-confirmed-by-local-authorities.xlsx
+++ b/cases-confirmed-by-local-authorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xshaun/GitHub/COVID-19-UK/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D869614-9F01-D848-9055-8AE3CB8ACCFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CEBD74E-A168-C548-A35B-FCC3766F603E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27720" windowHeight="17540" xr2:uid="{03FAC37E-E114-B94A-90DB-A205D9B9D727}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="165">
   <si>
     <t>Local authority</t>
   </si>
@@ -525,6 +525,9 @@
   </si>
   <si>
     <t>9:00am on 9 March 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9:00am on 10 March 2020</t>
   </si>
 </sst>
 </file>
@@ -905,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E24FA156-A3A6-9444-8142-DD1738F7E1B2}">
-  <dimension ref="A1:H155"/>
+  <dimension ref="A1:J155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:H155"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="I155" sqref="I155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -923,7 +926,7 @@
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -948,8 +951,11 @@
       <c r="H1" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J1" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -974,8 +980,14 @@
       <c r="H2" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1000,8 +1012,14 @@
       <c r="H3" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1026,8 +1044,14 @@
       <c r="H4" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1052,8 +1076,14 @@
       <c r="H5" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1078,8 +1108,14 @@
       <c r="H6" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1104,8 +1140,14 @@
       <c r="H7" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1130,8 +1172,14 @@
       <c r="H8" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1156,8 +1204,14 @@
       <c r="H9" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1182,8 +1236,14 @@
       <c r="H10" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1208,8 +1268,14 @@
       <c r="H11" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1234,8 +1300,14 @@
       <c r="H12" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I12" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J12" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1260,8 +1332,14 @@
       <c r="H13" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1286,8 +1364,14 @@
       <c r="H14" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1312,8 +1396,14 @@
       <c r="H15" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1338,8 +1428,14 @@
       <c r="H16" s="5">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -1364,8 +1460,14 @@
       <c r="H17" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -1390,8 +1492,14 @@
       <c r="H18" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
@@ -1416,8 +1524,14 @@
       <c r="H19" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -1442,8 +1556,14 @@
       <c r="H20" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
@@ -1468,8 +1588,14 @@
       <c r="H21" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
@@ -1494,8 +1620,14 @@
       <c r="H22" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
@@ -1520,8 +1652,14 @@
       <c r="H23" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J23" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
@@ -1546,8 +1684,14 @@
       <c r="H24" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>25</v>
       </c>
@@ -1572,8 +1716,14 @@
       <c r="H25" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
@@ -1598,8 +1748,14 @@
       <c r="H26" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>27</v>
       </c>
@@ -1616,8 +1772,14 @@
       <c r="H27" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I27" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="J27" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
@@ -1642,8 +1804,14 @@
       <c r="H28" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>29</v>
       </c>
@@ -1668,8 +1836,14 @@
       <c r="H29" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J29" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>30</v>
       </c>
@@ -1694,8 +1868,14 @@
       <c r="H30" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
@@ -1720,8 +1900,14 @@
       <c r="H31" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J31" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>32</v>
       </c>
@@ -1746,8 +1932,14 @@
       <c r="H32" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>33</v>
       </c>
@@ -1772,8 +1964,14 @@
       <c r="H33" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
@@ -1798,8 +1996,14 @@
       <c r="H34" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J34" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>35</v>
       </c>
@@ -1824,8 +2028,14 @@
       <c r="H35" s="5">
         <v>12</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J35" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>36</v>
       </c>
@@ -1850,8 +2060,14 @@
       <c r="H36" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>37</v>
       </c>
@@ -1876,8 +2092,14 @@
       <c r="H37" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>38</v>
       </c>
@@ -1902,8 +2124,14 @@
       <c r="H38" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>39</v>
       </c>
@@ -1928,8 +2156,14 @@
       <c r="H39" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J39" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>40</v>
       </c>
@@ -1954,8 +2188,14 @@
       <c r="H40" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I40" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>41</v>
       </c>
@@ -1980,8 +2220,14 @@
       <c r="H41" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I41" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J41" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>42</v>
       </c>
@@ -2006,8 +2252,14 @@
       <c r="H42" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I42" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>43</v>
       </c>
@@ -2032,8 +2284,14 @@
       <c r="H43" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I43" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J43" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>44</v>
       </c>
@@ -2058,8 +2316,14 @@
       <c r="H44" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I44" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>45</v>
       </c>
@@ -2084,8 +2348,14 @@
       <c r="H45" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I45" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J45" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>46</v>
       </c>
@@ -2110,8 +2380,14 @@
       <c r="H46" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I46" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>47</v>
       </c>
@@ -2136,8 +2412,14 @@
       <c r="H47" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I47" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="J47" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>48</v>
       </c>
@@ -2162,8 +2444,14 @@
       <c r="H48" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I48" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J48" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>49</v>
       </c>
@@ -2188,8 +2476,14 @@
       <c r="H49" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I49" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J49" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>50</v>
       </c>
@@ -2214,8 +2508,14 @@
       <c r="H50" s="5">
         <v>8</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I50" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J50" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>51</v>
       </c>
@@ -2240,8 +2540,14 @@
       <c r="H51" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I51" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J51" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>52</v>
       </c>
@@ -2266,8 +2572,14 @@
       <c r="H52" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I52" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J52" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>53</v>
       </c>
@@ -2292,8 +2604,14 @@
       <c r="H53" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I53" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J53" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>54</v>
       </c>
@@ -2318,8 +2636,14 @@
       <c r="H54" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I54" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J54" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>55</v>
       </c>
@@ -2344,8 +2668,14 @@
       <c r="H55" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I55" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>56</v>
       </c>
@@ -2370,8 +2700,14 @@
       <c r="H56" s="5">
         <v>13</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I56" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J56" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>57</v>
       </c>
@@ -2396,8 +2732,14 @@
       <c r="H57" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I57" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J57" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>58</v>
       </c>
@@ -2422,8 +2764,14 @@
       <c r="H58" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I58" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J58" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>59</v>
       </c>
@@ -2448,8 +2796,14 @@
       <c r="H59" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I59" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>60</v>
       </c>
@@ -2474,8 +2828,14 @@
       <c r="H60" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I60" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J60" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>61</v>
       </c>
@@ -2492,8 +2852,14 @@
       <c r="H61" s="5">
         <v>8</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I61" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J61" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>62</v>
       </c>
@@ -2518,8 +2884,14 @@
       <c r="H62" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I62" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J62" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>63</v>
       </c>
@@ -2544,8 +2916,14 @@
       <c r="H63" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I63" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J63" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>64</v>
       </c>
@@ -2570,8 +2948,14 @@
       <c r="H64" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I64" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J64" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>65</v>
       </c>
@@ -2596,8 +2980,14 @@
       <c r="H65" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I65" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J65" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>66</v>
       </c>
@@ -2622,8 +3012,14 @@
       <c r="H66" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I66" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J66" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>67</v>
       </c>
@@ -2648,8 +3044,14 @@
       <c r="H67" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I67" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J67" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>68</v>
       </c>
@@ -2674,8 +3076,14 @@
       <c r="H68" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I68" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J68" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>69</v>
       </c>
@@ -2700,8 +3108,14 @@
       <c r="H69" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I69" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J69" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>70</v>
       </c>
@@ -2726,8 +3140,14 @@
       <c r="H70" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I70" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J70" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>71</v>
       </c>
@@ -2752,8 +3172,14 @@
       <c r="H71" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I71" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J71" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>72</v>
       </c>
@@ -2778,8 +3204,14 @@
       <c r="H72" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I72" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J72" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>73</v>
       </c>
@@ -2804,8 +3236,14 @@
       <c r="H73" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I73" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J73" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>74</v>
       </c>
@@ -2830,8 +3268,14 @@
       <c r="H74" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I74" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J74" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>75</v>
       </c>
@@ -2856,8 +3300,14 @@
       <c r="H75" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I75" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J75" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>76</v>
       </c>
@@ -2882,8 +3332,14 @@
       <c r="H76" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I76" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J76" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>77</v>
       </c>
@@ -2908,8 +3364,14 @@
       <c r="H77" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I77" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J77" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>78</v>
       </c>
@@ -2934,8 +3396,14 @@
       <c r="H78" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I78" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J78" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>79</v>
       </c>
@@ -2960,8 +3428,14 @@
       <c r="H79" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I79" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J79" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>80</v>
       </c>
@@ -2986,8 +3460,14 @@
       <c r="H80" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I80" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="J80" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>81</v>
       </c>
@@ -3012,8 +3492,14 @@
       <c r="H81" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I81" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J81" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>82</v>
       </c>
@@ -3038,8 +3524,14 @@
       <c r="H82" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I82" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J82" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>83</v>
       </c>
@@ -3064,8 +3556,14 @@
       <c r="H83" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I83" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J83" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>84</v>
       </c>
@@ -3090,8 +3588,14 @@
       <c r="H84" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I84" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J84" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>85</v>
       </c>
@@ -3116,8 +3620,14 @@
       <c r="H85" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I85" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J85" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>86</v>
       </c>
@@ -3142,8 +3652,14 @@
       <c r="H86" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I86" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J86" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>87</v>
       </c>
@@ -3168,8 +3684,14 @@
       <c r="H87" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I87" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J87" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>88</v>
       </c>
@@ -3194,8 +3716,14 @@
       <c r="H88" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I88" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J88" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>89</v>
       </c>
@@ -3220,8 +3748,14 @@
       <c r="H89" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I89" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J89" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>90</v>
       </c>
@@ -3246,8 +3780,14 @@
       <c r="H90" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I90" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J90" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>91</v>
       </c>
@@ -3272,8 +3812,14 @@
       <c r="H91" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I91" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J91" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>92</v>
       </c>
@@ -3298,8 +3844,14 @@
       <c r="H92" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I92" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J92" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>93</v>
       </c>
@@ -3324,8 +3876,14 @@
       <c r="H93" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I93" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J93" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>94</v>
       </c>
@@ -3350,8 +3908,14 @@
       <c r="H94" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I94" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J94" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>95</v>
       </c>
@@ -3376,8 +3940,14 @@
       <c r="H95" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I95" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J95" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>96</v>
       </c>
@@ -3402,8 +3972,14 @@
       <c r="H96" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I96" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J96" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>97</v>
       </c>
@@ -3428,8 +4004,14 @@
       <c r="H97" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I97" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J97" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>98</v>
       </c>
@@ -3454,8 +4036,14 @@
       <c r="H98" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I98" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J98" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>99</v>
       </c>
@@ -3476,8 +4064,14 @@
       <c r="H99" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I99" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J99" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>100</v>
       </c>
@@ -3502,8 +4096,14 @@
       <c r="H100" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I100" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J100" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>101</v>
       </c>
@@ -3528,8 +4128,14 @@
       <c r="H101" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I101" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J101" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>102</v>
       </c>
@@ -3554,8 +4160,14 @@
       <c r="H102" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I102" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J102" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>103</v>
       </c>
@@ -3580,8 +4192,14 @@
       <c r="H103" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I103" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J103" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>104</v>
       </c>
@@ -3606,8 +4224,14 @@
       <c r="H104" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I104" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J104" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>105</v>
       </c>
@@ -3632,8 +4256,14 @@
       <c r="H105" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I105" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J105" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>106</v>
       </c>
@@ -3658,8 +4288,14 @@
       <c r="H106" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I106" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J106" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>107</v>
       </c>
@@ -3684,8 +4320,14 @@
       <c r="H107" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I107" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J107" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>108</v>
       </c>
@@ -3710,8 +4352,14 @@
       <c r="H108" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I108" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J108" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>109</v>
       </c>
@@ -3736,8 +4384,14 @@
       <c r="H109" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I109" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J109" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>110</v>
       </c>
@@ -3762,8 +4416,14 @@
       <c r="H110" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I110" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J110" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>111</v>
       </c>
@@ -3788,8 +4448,14 @@
       <c r="H111" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I111" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J111" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>112</v>
       </c>
@@ -3814,8 +4480,14 @@
       <c r="H112" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I112" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="J112" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>113</v>
       </c>
@@ -3840,8 +4512,14 @@
       <c r="H113" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I113" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J113" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>114</v>
       </c>
@@ -3866,8 +4544,14 @@
       <c r="H114" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I114" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J114" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>115</v>
       </c>
@@ -3892,8 +4576,14 @@
       <c r="H115" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I115" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J115" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>116</v>
       </c>
@@ -3918,8 +4608,14 @@
       <c r="H116" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I116" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J116" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>117</v>
       </c>
@@ -3944,8 +4640,14 @@
       <c r="H117" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I117" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J117" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>118</v>
       </c>
@@ -3970,8 +4672,14 @@
       <c r="H118" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I118" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J118" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>119</v>
       </c>
@@ -3996,8 +4704,14 @@
       <c r="H119" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I119" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J119" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>120</v>
       </c>
@@ -4022,8 +4736,14 @@
       <c r="H120" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I120" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J120" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>121</v>
       </c>
@@ -4048,8 +4768,14 @@
       <c r="H121" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I121" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J121" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>122</v>
       </c>
@@ -4074,8 +4800,14 @@
       <c r="H122" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I122" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="J122" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>123</v>
       </c>
@@ -4100,8 +4832,14 @@
       <c r="H123" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I123" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J123" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>124</v>
       </c>
@@ -4126,8 +4864,14 @@
       <c r="H124" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I124" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J124" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>125</v>
       </c>
@@ -4152,8 +4896,14 @@
       <c r="H125" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I125" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J125" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>126</v>
       </c>
@@ -4178,8 +4928,14 @@
       <c r="H126" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I126" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J126" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>127</v>
       </c>
@@ -4204,8 +4960,14 @@
       <c r="H127" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I127" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="J127" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>128</v>
       </c>
@@ -4230,8 +4992,14 @@
       <c r="H128" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I128" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="J128" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>129</v>
       </c>
@@ -4256,8 +5024,14 @@
       <c r="H129" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I129" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J129" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>130</v>
       </c>
@@ -4282,8 +5056,14 @@
       <c r="H130" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I130" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="J130" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>131</v>
       </c>
@@ -4308,8 +5088,14 @@
       <c r="H131" s="5">
         <v>7</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I131" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="J131" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>132</v>
       </c>
@@ -4334,8 +5120,14 @@
       <c r="H132" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I132" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J132" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>133</v>
       </c>
@@ -4360,8 +5152,14 @@
       <c r="H133" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="134" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I133" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J133" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>134</v>
       </c>
@@ -4386,8 +5184,14 @@
       <c r="H134" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I134" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J134" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>135</v>
       </c>
@@ -4412,8 +5216,14 @@
       <c r="H135" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I135" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="J135" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>136</v>
       </c>
@@ -4438,8 +5248,14 @@
       <c r="H136" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="137" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I136" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="J136" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>137</v>
       </c>
@@ -4464,8 +5280,14 @@
       <c r="H137" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="138" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I137" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J137" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>138</v>
       </c>
@@ -4490,8 +5312,14 @@
       <c r="H138" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I138" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J138" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>139</v>
       </c>
@@ -4516,8 +5344,14 @@
       <c r="H139" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="140" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I139" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J139" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>140</v>
       </c>
@@ -4542,8 +5376,14 @@
       <c r="H140" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I140" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="J140" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>141</v>
       </c>
@@ -4568,8 +5408,14 @@
       <c r="H141" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="142" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I141" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="J141" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>142</v>
       </c>
@@ -4594,8 +5440,14 @@
       <c r="H142" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="143" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I142" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="J142" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>143</v>
       </c>
@@ -4620,8 +5472,14 @@
       <c r="H143" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="144" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I143" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J143" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>144</v>
       </c>
@@ -4646,8 +5504,14 @@
       <c r="H144" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="145" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I144" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="J144" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>145</v>
       </c>
@@ -4672,8 +5536,14 @@
       <c r="H145" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I145" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="J145" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>146</v>
       </c>
@@ -4698,8 +5568,14 @@
       <c r="H146" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="147" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I146" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="J146" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>147</v>
       </c>
@@ -4724,8 +5600,14 @@
       <c r="H147" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="148" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I147" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="J147" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>148</v>
       </c>
@@ -4750,8 +5632,14 @@
       <c r="H148" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="149" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I148" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="J148" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>149</v>
       </c>
@@ -4776,8 +5664,14 @@
       <c r="H149" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="150" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I149" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="J149" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>150</v>
       </c>
@@ -4802,8 +5696,14 @@
       <c r="H150" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="151" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I150" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J150" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>151</v>
       </c>
@@ -4828,8 +5728,14 @@
       <c r="H151" s="5">
         <v>26</v>
       </c>
-    </row>
-    <row r="152" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I151" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J151" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>152</v>
       </c>
@@ -4849,7 +5755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>153</v>
       </c>
@@ -4869,7 +5775,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="154" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>154</v>
       </c>
@@ -4889,7 +5795,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155" s="3"/>
       <c r="B155" s="3"/>
       <c r="C155" s="3"/>

</xml_diff>